<commit_message>
Updated Auto_Stocks.xlsx with new data
</commit_message>
<xml_diff>
--- a/NAV/Auto_Stocks.xlsx
+++ b/NAV/Auto_Stocks.xlsx
@@ -502,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J595"/>
+  <dimension ref="A1:J612"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A584" workbookViewId="0">
       <selection activeCell="E612" sqref="E612"/>
@@ -18939,8 +18939,595 @@
         <v>276.6255023403813</v>
       </c>
     </row>
-    <row r="594"/>
-    <row r="595"/>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>2024-08-28</t>
+        </is>
+      </c>
+      <c r="C594" t="n">
+        <v>1074.550048828125</v>
+      </c>
+      <c r="D594" t="n">
+        <v>700.0999755859375</v>
+      </c>
+      <c r="E594" t="n">
+        <v>260.4500122070312</v>
+      </c>
+      <c r="F594" t="n">
+        <v>491.7000122070312</v>
+      </c>
+      <c r="G594" t="n">
+        <v>1535.849975585938</v>
+      </c>
+      <c r="H594" t="n">
+        <v>29293.15045166016</v>
+      </c>
+      <c r="I594" t="n">
+        <v>-0.009101137231307158</v>
+      </c>
+      <c r="J594" t="n">
+        <v>274.1078956819022</v>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>2024-08-29</t>
+        </is>
+      </c>
+      <c r="C595" t="n">
+        <v>1121.650024414062</v>
+      </c>
+      <c r="D595" t="n">
+        <v>689.1500244140625</v>
+      </c>
+      <c r="E595" t="n">
+        <v>253.8000030517578</v>
+      </c>
+      <c r="F595" t="n">
+        <v>490.2000122070312</v>
+      </c>
+      <c r="G595" t="n">
+        <v>1520.25</v>
+      </c>
+      <c r="H595" t="n">
+        <v>29353.35063171387</v>
+      </c>
+      <c r="I595" t="n">
+        <v>0.002055094079179154</v>
+      </c>
+      <c r="J595" t="n">
+        <v>274.6712131953744</v>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>2024-08-30</t>
+        </is>
+      </c>
+      <c r="C596" t="n">
+        <v>1111.349975585938</v>
+      </c>
+      <c r="D596" t="n">
+        <v>683.3499755859375</v>
+      </c>
+      <c r="E596" t="n">
+        <v>256.4500122070312</v>
+      </c>
+      <c r="F596" t="n">
+        <v>492.8999938964844</v>
+      </c>
+      <c r="G596" t="n">
+        <v>1521</v>
+      </c>
+      <c r="H596" t="n">
+        <v>29291.19976806641</v>
+      </c>
+      <c r="I596" t="n">
+        <v>-0.002117334556700047</v>
+      </c>
+      <c r="J596" t="n">
+        <v>274.0896423439451</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>2024-09-02</t>
+        </is>
+      </c>
+      <c r="C597" t="n">
+        <v>1092.650024414062</v>
+      </c>
+      <c r="D597" t="n">
+        <v>715.0499877929688</v>
+      </c>
+      <c r="E597" t="n">
+        <v>251.3500061035156</v>
+      </c>
+      <c r="F597" t="n">
+        <v>490.5</v>
+      </c>
+      <c r="G597" t="n">
+        <v>1505.25</v>
+      </c>
+      <c r="H597" t="n">
+        <v>29322.30020141602</v>
+      </c>
+      <c r="I597" t="n">
+        <v>0.00106176713811209</v>
+      </c>
+      <c r="J597" t="n">
+        <v>274.3806617190828</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>2024-09-03</t>
+        </is>
+      </c>
+      <c r="C598" t="n">
+        <v>1085.099975585938</v>
+      </c>
+      <c r="D598" t="n">
+        <v>710.7999877929688</v>
+      </c>
+      <c r="E598" t="n">
+        <v>251</v>
+      </c>
+      <c r="F598" t="n">
+        <v>488.8500061035156</v>
+      </c>
+      <c r="G598" t="n">
+        <v>1509</v>
+      </c>
+      <c r="H598" t="n">
+        <v>29201.39971923828</v>
+      </c>
+      <c r="I598" t="n">
+        <v>-0.004123158188384413</v>
+      </c>
+      <c r="J598" t="n">
+        <v>273.2493468469814</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>2024-09-04</t>
+        </is>
+      </c>
+      <c r="C599" t="n">
+        <v>1080.449951171875</v>
+      </c>
+      <c r="D599" t="n">
+        <v>722.4000244140625</v>
+      </c>
+      <c r="E599" t="n">
+        <v>250.5</v>
+      </c>
+      <c r="F599" t="n">
+        <v>484.1499938964844</v>
+      </c>
+      <c r="G599" t="n">
+        <v>1488.099975585938</v>
+      </c>
+      <c r="H599" t="n">
+        <v>29200.89978027344</v>
+      </c>
+      <c r="I599" t="n">
+        <v>-1.712037675078922e-05</v>
+      </c>
+      <c r="J599" t="n">
+        <v>273.2446687152164</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>2024-09-05</t>
+        </is>
+      </c>
+      <c r="C600" t="n">
+        <v>1069.150024414062</v>
+      </c>
+      <c r="D600" t="n">
+        <v>733.8499755859375</v>
+      </c>
+      <c r="E600" t="n">
+        <v>251.1499938964844</v>
+      </c>
+      <c r="F600" t="n">
+        <v>495.6499938964844</v>
+      </c>
+      <c r="G600" t="n">
+        <v>1447.599975585938</v>
+      </c>
+      <c r="H600" t="n">
+        <v>29262.3996887207</v>
+      </c>
+      <c r="I600" t="n">
+        <v>0.002106096350113556</v>
+      </c>
+      <c r="J600" t="n">
+        <v>273.8201483146856</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>2024-09-06</t>
+        </is>
+      </c>
+      <c r="C601" t="n">
+        <v>1049.349975585938</v>
+      </c>
+      <c r="D601" t="n">
+        <v>718.9000244140625</v>
+      </c>
+      <c r="E601" t="n">
+        <v>247.8000030517578</v>
+      </c>
+      <c r="F601" t="n">
+        <v>483</v>
+      </c>
+      <c r="G601" t="n">
+        <v>1418.050048828125</v>
+      </c>
+      <c r="H601" t="n">
+        <v>28702.20024108887</v>
+      </c>
+      <c r="I601" t="n">
+        <v>-0.01914400232349252</v>
+      </c>
+      <c r="J601" t="n">
+        <v>268.5781347591301</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="C602" t="n">
+        <v>1038.699951171875</v>
+      </c>
+      <c r="D602" t="n">
+        <v>700.1500244140625</v>
+      </c>
+      <c r="E602" t="n">
+        <v>243.8999938964844</v>
+      </c>
+      <c r="F602" t="n">
+        <v>474.75</v>
+      </c>
+      <c r="G602" t="n">
+        <v>1411.849975585938</v>
+      </c>
+      <c r="H602" t="n">
+        <v>28242.6496887207</v>
+      </c>
+      <c r="I602" t="n">
+        <v>-0.01601098691069303</v>
+      </c>
+      <c r="J602" t="n">
+        <v>264.2779337590034</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>2024-09-10</t>
+        </is>
+      </c>
+      <c r="C603" t="n">
+        <v>1035.800048828125</v>
+      </c>
+      <c r="D603" t="n">
+        <v>713.4000244140625</v>
+      </c>
+      <c r="E603" t="n">
+        <v>248.25</v>
+      </c>
+      <c r="F603" t="n">
+        <v>478.7999877929688</v>
+      </c>
+      <c r="G603" t="n">
+        <v>1424.449951171875</v>
+      </c>
+      <c r="H603" t="n">
+        <v>28522.85046386719</v>
+      </c>
+      <c r="I603" t="n">
+        <v>0.009921192885042528</v>
+      </c>
+      <c r="J603" t="n">
+        <v>266.8998861150869</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>2024-09-11</t>
+        </is>
+      </c>
+      <c r="C604" t="n">
+        <v>976.2999877929688</v>
+      </c>
+      <c r="D604" t="n">
+        <v>725.4000244140625</v>
+      </c>
+      <c r="E604" t="n">
+        <v>241.5500030517578</v>
+      </c>
+      <c r="F604" t="n">
+        <v>472.2000122070312</v>
+      </c>
+      <c r="G604" t="n">
+        <v>1399.599975585938</v>
+      </c>
+      <c r="H604" t="n">
+        <v>27922.25028991699</v>
+      </c>
+      <c r="I604" t="n">
+        <v>-0.02105680758348599</v>
+      </c>
+      <c r="J604" t="n">
+        <v>261.2798265691072</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="C605" t="n">
+        <v>986.1500244140625</v>
+      </c>
+      <c r="D605" t="n">
+        <v>726.0499877929688</v>
+      </c>
+      <c r="E605" t="n">
+        <v>246.1499938964844</v>
+      </c>
+      <c r="F605" t="n">
+        <v>479.8500061035156</v>
+      </c>
+      <c r="G605" t="n">
+        <v>1403.150024414062</v>
+      </c>
+      <c r="H605" t="n">
+        <v>28182.30001831055</v>
+      </c>
+      <c r="I605" t="n">
+        <v>0.009313351384414074</v>
+      </c>
+      <c r="J605" t="n">
+        <v>263.7132174036041</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="C606" t="n">
+        <v>992.0999755859375</v>
+      </c>
+      <c r="D606" t="n">
+        <v>724.25</v>
+      </c>
+      <c r="E606" t="n">
+        <v>245.6499938964844</v>
+      </c>
+      <c r="F606" t="n">
+        <v>485.3999938964844</v>
+      </c>
+      <c r="G606" t="n">
+        <v>1410.949951171875</v>
+      </c>
+      <c r="H606" t="n">
+        <v>28258.59951782227</v>
+      </c>
+      <c r="I606" t="n">
+        <v>0.002707355306775728</v>
+      </c>
+      <c r="J606" t="n">
+        <v>264.4271827822087</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>2024-09-16</t>
+        </is>
+      </c>
+      <c r="C607" t="n">
+        <v>988.4000244140625</v>
+      </c>
+      <c r="D607" t="n">
+        <v>733.6500244140625</v>
+      </c>
+      <c r="E607" t="n">
+        <v>243.8000030517578</v>
+      </c>
+      <c r="F607" t="n">
+        <v>489.9500122070312</v>
+      </c>
+      <c r="G607" t="n">
+        <v>1404.550048828125</v>
+      </c>
+      <c r="H607" t="n">
+        <v>28313.45072937012</v>
+      </c>
+      <c r="I607" t="n">
+        <v>0.00194104493795801</v>
+      </c>
+      <c r="J607" t="n">
+        <v>264.9404478268066</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>2024-09-17</t>
+        </is>
+      </c>
+      <c r="C608" t="n">
+        <v>974.9500122070312</v>
+      </c>
+      <c r="D608" t="n">
+        <v>745.4000244140625</v>
+      </c>
+      <c r="E608" t="n">
+        <v>240.8000030517578</v>
+      </c>
+      <c r="F608" t="n">
+        <v>482.2999877929688</v>
+      </c>
+      <c r="G608" t="n">
+        <v>1400.25</v>
+      </c>
+      <c r="H608" t="n">
+        <v>28196.30033874512</v>
+      </c>
+      <c r="I608" t="n">
+        <v>-0.004137623200533361</v>
+      </c>
+      <c r="J608" t="n">
+        <v>263.8442240831187</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>2024-09-18</t>
+        </is>
+      </c>
+      <c r="C609" t="n">
+        <v>962.0499877929688</v>
+      </c>
+      <c r="D609" t="n">
+        <v>717.5499877929688</v>
+      </c>
+      <c r="E609" t="n">
+        <v>235.9499969482422</v>
+      </c>
+      <c r="F609" t="n">
+        <v>471.75</v>
+      </c>
+      <c r="G609" t="n">
+        <v>1391.300048828125</v>
+      </c>
+      <c r="H609" t="n">
+        <v>27572.89979553223</v>
+      </c>
+      <c r="I609" t="n">
+        <v>-0.02210930284198537</v>
+      </c>
+      <c r="J609" t="n">
+        <v>258.0108122297563</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>2024-09-19</t>
+        </is>
+      </c>
+      <c r="C610" t="n">
+        <v>967</v>
+      </c>
+      <c r="D610" t="n">
+        <v>728.5</v>
+      </c>
+      <c r="E610" t="n">
+        <v>237.5500030517578</v>
+      </c>
+      <c r="F610" t="n">
+        <v>459.9500122070312</v>
+      </c>
+      <c r="G610" t="n">
+        <v>1374.150024414062</v>
+      </c>
+      <c r="H610" t="n">
+        <v>27641.0502166748</v>
+      </c>
+      <c r="I610" t="n">
+        <v>0.002471645044516532</v>
+      </c>
+      <c r="J610" t="n">
+        <v>258.6485233752357</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
+      <c r="C611" t="n">
+        <v>970.8499755859375</v>
+      </c>
+      <c r="D611" t="n">
+        <v>748.3499755859375</v>
+      </c>
+      <c r="E611" t="n">
+        <v>237.8500061035156</v>
+      </c>
+      <c r="F611" t="n">
+        <v>466.2999877929688</v>
+      </c>
+      <c r="G611" t="n">
+        <v>1380.550048828125</v>
+      </c>
+      <c r="H611" t="n">
+        <v>27960.69967651367</v>
+      </c>
+      <c r="I611" t="n">
+        <v>0.01156430227264067</v>
+      </c>
+      <c r="J611" t="n">
+        <v>261.6396130819191</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="C612" t="n">
+        <v>971.7999877929688</v>
+      </c>
+      <c r="D612" t="n">
+        <v>750.2000122070312</v>
+      </c>
+      <c r="E612" t="n">
+        <v>236.4499969482422</v>
+      </c>
+      <c r="F612" t="n">
+        <v>471.1499938964844</v>
+      </c>
+      <c r="G612" t="n">
+        <v>1375.400024414062</v>
+      </c>
+      <c r="H612" t="n">
+        <v>27984.94996643066</v>
+      </c>
+      <c r="I612" t="n">
+        <v>0.0008672991090191444</v>
+      </c>
+      <c r="J612" t="n">
+        <v>261.8665328852292</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Capital_Goods.xlsx, Auto_Stocks.xlsx, FMCG_stocks.xlsx, Large_Caps.xlsx, Luxury_Goods.xlsx, Pharma_stocks.xlsx, IT_Stocks.xlsx with new data
</commit_message>
<xml_diff>
--- a/NAV/Auto_Stocks.xlsx
+++ b/NAV/Auto_Stocks.xlsx
@@ -502,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J633"/>
+  <dimension ref="A1:J653"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A584" workbookViewId="0">
       <selection activeCell="E612" sqref="E612"/>
@@ -20179,6 +20179,626 @@
         <v>257.7896181747883</v>
       </c>
     </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>2024-09-02</t>
+        </is>
+      </c>
+      <c r="C634" t="n">
+        <v>1092.650024414062</v>
+      </c>
+      <c r="D634" t="n">
+        <v>715.0499877929688</v>
+      </c>
+      <c r="E634" t="n">
+        <v>251.3500061035156</v>
+      </c>
+      <c r="F634" t="n">
+        <v>490.5</v>
+      </c>
+      <c r="G634" t="n">
+        <v>1505.25</v>
+      </c>
+      <c r="H634" t="n">
+        <v>29322.30020141602</v>
+      </c>
+      <c r="I634" t="n">
+        <v>0</v>
+      </c>
+      <c r="J634" t="n">
+        <v>257.7896181747883</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>2024-09-03</t>
+        </is>
+      </c>
+      <c r="C635" t="n">
+        <v>1085.099975585938</v>
+      </c>
+      <c r="D635" t="n">
+        <v>710.7999877929688</v>
+      </c>
+      <c r="E635" t="n">
+        <v>251</v>
+      </c>
+      <c r="F635" t="n">
+        <v>488.8500061035156</v>
+      </c>
+      <c r="G635" t="n">
+        <v>1509</v>
+      </c>
+      <c r="H635" t="n">
+        <v>29201.39971923828</v>
+      </c>
+      <c r="I635" t="n">
+        <v>-0.004123158188384413</v>
+      </c>
+      <c r="J635" t="n">
+        <v>256.7267107997304</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>2024-09-04</t>
+        </is>
+      </c>
+      <c r="C636" t="n">
+        <v>1080.449951171875</v>
+      </c>
+      <c r="D636" t="n">
+        <v>722.4000244140625</v>
+      </c>
+      <c r="E636" t="n">
+        <v>250.5</v>
+      </c>
+      <c r="F636" t="n">
+        <v>484.1499938964844</v>
+      </c>
+      <c r="G636" t="n">
+        <v>1488.099975585938</v>
+      </c>
+      <c r="H636" t="n">
+        <v>29200.89978027344</v>
+      </c>
+      <c r="I636" t="n">
+        <v>-1.712037675078922e-05</v>
+      </c>
+      <c r="J636" t="n">
+        <v>256.7223155417195</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>2024-09-05</t>
+        </is>
+      </c>
+      <c r="C637" t="n">
+        <v>1069.150024414062</v>
+      </c>
+      <c r="D637" t="n">
+        <v>733.8499755859375</v>
+      </c>
+      <c r="E637" t="n">
+        <v>251.1499938964844</v>
+      </c>
+      <c r="F637" t="n">
+        <v>495.6499938964844</v>
+      </c>
+      <c r="G637" t="n">
+        <v>1447.599975585938</v>
+      </c>
+      <c r="H637" t="n">
+        <v>29262.3996887207</v>
+      </c>
+      <c r="I637" t="n">
+        <v>0.002106096350113556</v>
+      </c>
+      <c r="J637" t="n">
+        <v>257.2629974734746</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>2024-09-06</t>
+        </is>
+      </c>
+      <c r="C638" t="n">
+        <v>1049.349975585938</v>
+      </c>
+      <c r="D638" t="n">
+        <v>718.9000244140625</v>
+      </c>
+      <c r="E638" t="n">
+        <v>247.8000030517578</v>
+      </c>
+      <c r="F638" t="n">
+        <v>483</v>
+      </c>
+      <c r="G638" t="n">
+        <v>1418.050048828125</v>
+      </c>
+      <c r="H638" t="n">
+        <v>28702.20024108887</v>
+      </c>
+      <c r="I638" t="n">
+        <v>-0.01914400232349252</v>
+      </c>
+      <c r="J638" t="n">
+        <v>252.3379540520938</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="C639" t="n">
+        <v>1038.699951171875</v>
+      </c>
+      <c r="D639" t="n">
+        <v>700.1500244140625</v>
+      </c>
+      <c r="E639" t="n">
+        <v>243.8999938964844</v>
+      </c>
+      <c r="F639" t="n">
+        <v>474.75</v>
+      </c>
+      <c r="G639" t="n">
+        <v>1411.849975585938</v>
+      </c>
+      <c r="H639" t="n">
+        <v>28242.6496887207</v>
+      </c>
+      <c r="I639" t="n">
+        <v>-0.01601098691069303</v>
+      </c>
+      <c r="J639" t="n">
+        <v>248.2977743726946</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>2024-09-10</t>
+        </is>
+      </c>
+      <c r="C640" t="n">
+        <v>1035.800048828125</v>
+      </c>
+      <c r="D640" t="n">
+        <v>713.4000244140625</v>
+      </c>
+      <c r="E640" t="n">
+        <v>248.25</v>
+      </c>
+      <c r="F640" t="n">
+        <v>478.7999877929688</v>
+      </c>
+      <c r="G640" t="n">
+        <v>1424.449951171875</v>
+      </c>
+      <c r="H640" t="n">
+        <v>28522.85046386719</v>
+      </c>
+      <c r="I640" t="n">
+        <v>0.009921192885042528</v>
+      </c>
+      <c r="J640" t="n">
+        <v>250.7611844851729</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>2024-09-11</t>
+        </is>
+      </c>
+      <c r="C641" t="n">
+        <v>976.2999877929688</v>
+      </c>
+      <c r="D641" t="n">
+        <v>725.4000244140625</v>
+      </c>
+      <c r="E641" t="n">
+        <v>241.5500030517578</v>
+      </c>
+      <c r="F641" t="n">
+        <v>472.2000122070312</v>
+      </c>
+      <c r="G641" t="n">
+        <v>1399.599975585938</v>
+      </c>
+      <c r="H641" t="n">
+        <v>27922.25028991699</v>
+      </c>
+      <c r="I641" t="n">
+        <v>-0.02105680758348599</v>
+      </c>
+      <c r="J641" t="n">
+        <v>245.4809544740616</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="C642" t="n">
+        <v>986.1500244140625</v>
+      </c>
+      <c r="D642" t="n">
+        <v>726.0499877929688</v>
+      </c>
+      <c r="E642" t="n">
+        <v>246.1499938964844</v>
+      </c>
+      <c r="F642" t="n">
+        <v>479.8500061035156</v>
+      </c>
+      <c r="G642" t="n">
+        <v>1403.150024414062</v>
+      </c>
+      <c r="H642" t="n">
+        <v>28182.30001831055</v>
+      </c>
+      <c r="I642" t="n">
+        <v>0.009313351384414074</v>
+      </c>
+      <c r="J642" t="n">
+        <v>247.7672048612599</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="C643" t="n">
+        <v>992.0999755859375</v>
+      </c>
+      <c r="D643" t="n">
+        <v>724.25</v>
+      </c>
+      <c r="E643" t="n">
+        <v>245.6499938964844</v>
+      </c>
+      <c r="F643" t="n">
+        <v>485.3999938964844</v>
+      </c>
+      <c r="G643" t="n">
+        <v>1410.949951171875</v>
+      </c>
+      <c r="H643" t="n">
+        <v>28258.59951782227</v>
+      </c>
+      <c r="I643" t="n">
+        <v>0.002707355306775728</v>
+      </c>
+      <c r="J643" t="n">
+        <v>248.437998718186</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>2024-09-16</t>
+        </is>
+      </c>
+      <c r="C644" t="n">
+        <v>988.4000244140625</v>
+      </c>
+      <c r="D644" t="n">
+        <v>733.6500244140625</v>
+      </c>
+      <c r="E644" t="n">
+        <v>243.8000030517578</v>
+      </c>
+      <c r="F644" t="n">
+        <v>489.9500122070312</v>
+      </c>
+      <c r="G644" t="n">
+        <v>1404.550048828125</v>
+      </c>
+      <c r="H644" t="n">
+        <v>28313.45072937012</v>
+      </c>
+      <c r="I644" t="n">
+        <v>0.00194104493795801</v>
+      </c>
+      <c r="J644" t="n">
+        <v>248.9202280379943</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>2024-09-17</t>
+        </is>
+      </c>
+      <c r="C645" t="n">
+        <v>974.9500122070312</v>
+      </c>
+      <c r="D645" t="n">
+        <v>745.4000244140625</v>
+      </c>
+      <c r="E645" t="n">
+        <v>240.8000030517578</v>
+      </c>
+      <c r="F645" t="n">
+        <v>482.2999877929688</v>
+      </c>
+      <c r="G645" t="n">
+        <v>1400.25</v>
+      </c>
+      <c r="H645" t="n">
+        <v>28196.30033874512</v>
+      </c>
+      <c r="I645" t="n">
+        <v>-0.004137623200533361</v>
+      </c>
+      <c r="J645" t="n">
+        <v>247.8902899273823</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>2024-09-18</t>
+        </is>
+      </c>
+      <c r="C646" t="n">
+        <v>962.0499877929688</v>
+      </c>
+      <c r="D646" t="n">
+        <v>717.5499877929688</v>
+      </c>
+      <c r="E646" t="n">
+        <v>235.9499969482422</v>
+      </c>
+      <c r="F646" t="n">
+        <v>471.75</v>
+      </c>
+      <c r="G646" t="n">
+        <v>1391.300048828125</v>
+      </c>
+      <c r="H646" t="n">
+        <v>27572.89979553223</v>
+      </c>
+      <c r="I646" t="n">
+        <v>-0.02210930284198537</v>
+      </c>
+      <c r="J646" t="n">
+        <v>242.4096084357902</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>2024-09-19</t>
+        </is>
+      </c>
+      <c r="C647" t="n">
+        <v>967</v>
+      </c>
+      <c r="D647" t="n">
+        <v>728.5</v>
+      </c>
+      <c r="E647" t="n">
+        <v>237.5500030517578</v>
+      </c>
+      <c r="F647" t="n">
+        <v>459.9500122070312</v>
+      </c>
+      <c r="G647" t="n">
+        <v>1374.150024414062</v>
+      </c>
+      <c r="H647" t="n">
+        <v>27641.0502166748</v>
+      </c>
+      <c r="I647" t="n">
+        <v>0.002471645044516532</v>
+      </c>
+      <c r="J647" t="n">
+        <v>243.0087589432238</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
+      <c r="C648" t="n">
+        <v>970.8499755859375</v>
+      </c>
+      <c r="D648" t="n">
+        <v>748.3499755859375</v>
+      </c>
+      <c r="E648" t="n">
+        <v>237.8500061035156</v>
+      </c>
+      <c r="F648" t="n">
+        <v>466.2999877929688</v>
+      </c>
+      <c r="G648" t="n">
+        <v>1380.550048828125</v>
+      </c>
+      <c r="H648" t="n">
+        <v>27960.69967651367</v>
+      </c>
+      <c r="I648" t="n">
+        <v>0.01156430227264067</v>
+      </c>
+      <c r="J648" t="n">
+        <v>245.8189856865425</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="C649" t="n">
+        <v>971.7999877929688</v>
+      </c>
+      <c r="D649" t="n">
+        <v>750.2000122070312</v>
+      </c>
+      <c r="E649" t="n">
+        <v>236.4499969482422</v>
+      </c>
+      <c r="F649" t="n">
+        <v>471.1499938964844</v>
+      </c>
+      <c r="G649" t="n">
+        <v>1375.400024414062</v>
+      </c>
+      <c r="H649" t="n">
+        <v>27984.94996643066</v>
+      </c>
+      <c r="I649" t="n">
+        <v>0.0008672991090191444</v>
+      </c>
+      <c r="J649" t="n">
+        <v>246.0321842738084</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="C650" t="n">
+        <v>977.2999877929688</v>
+      </c>
+      <c r="D650" t="n">
+        <v>735.9000244140625</v>
+      </c>
+      <c r="E650" t="n">
+        <v>237.3000030517578</v>
+      </c>
+      <c r="F650" t="n">
+        <v>476.7000122070312</v>
+      </c>
+      <c r="G650" t="n">
+        <v>1363.699951171875</v>
+      </c>
+      <c r="H650" t="n">
+        <v>27912.20024108887</v>
+      </c>
+      <c r="I650" t="n">
+        <v>-0.002599601765558408</v>
+      </c>
+      <c r="J650" t="n">
+        <v>245.392598573186</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>2024-09-25</t>
+        </is>
+      </c>
+      <c r="C651" t="n">
+        <v>963.5999755859375</v>
+      </c>
+      <c r="D651" t="n">
+        <v>730.0499877929688</v>
+      </c>
+      <c r="E651" t="n">
+        <v>238.3500061035156</v>
+      </c>
+      <c r="F651" t="n">
+        <v>473.7000122070312</v>
+      </c>
+      <c r="G651" t="n">
+        <v>1365.400024414062</v>
+      </c>
+      <c r="H651" t="n">
+        <v>27741.79995727539</v>
+      </c>
+      <c r="I651" t="n">
+        <v>-0.006104867489544392</v>
+      </c>
+      <c r="J651" t="n">
+        <v>243.8945092759817</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>2024-09-26</t>
+        </is>
+      </c>
+      <c r="C652" t="n">
+        <v>993.1500244140625</v>
+      </c>
+      <c r="D652" t="n">
+        <v>744.0999755859375</v>
+      </c>
+      <c r="E652" t="n">
+        <v>241.1999969482422</v>
+      </c>
+      <c r="F652" t="n">
+        <v>471.75</v>
+      </c>
+      <c r="G652" t="n">
+        <v>1329.949951171875</v>
+      </c>
+      <c r="H652" t="n">
+        <v>28111.79975891113</v>
+      </c>
+      <c r="I652" t="n">
+        <v>0.01333726730801793</v>
+      </c>
+      <c r="J652" t="n">
+        <v>247.1473955411533</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>2024-09-27</t>
+        </is>
+      </c>
+      <c r="C653" t="n">
+        <v>993</v>
+      </c>
+      <c r="D653" t="n">
+        <v>735.4500122070312</v>
+      </c>
+      <c r="E653" t="n">
+        <v>239.5500030517578</v>
+      </c>
+      <c r="F653" t="n">
+        <v>497.2999877929688</v>
+      </c>
+      <c r="G653" t="n">
+        <v>1392.199951171875</v>
+      </c>
+      <c r="H653" t="n">
+        <v>28306.40000915527</v>
+      </c>
+      <c r="I653" t="n">
+        <v>0.006922368966521059</v>
+      </c>
+      <c r="J653" t="n">
+        <v>248.8582410022039</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Pharma_stocks.xlsx, FMCG_stocks.xlsx, Capital_Goods.xlsx, Large_Caps.xlsx, IT_Stocks.xlsx, Auto_Stocks.xlsx, Luxury_Goods.xlsx with new data
</commit_message>
<xml_diff>
--- a/NAV/Auto_Stocks.xlsx
+++ b/NAV/Auto_Stocks.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-1400" yWindow="2720" windowWidth="28040" windowHeight="16940" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -535,7 +535,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K700"/>
+  <dimension ref="A1:K759"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A641" workbookViewId="0">
       <selection activeCell="I656" sqref="I656"/>
@@ -22094,6 +22094,1717 @@
         <v>197.2977129751083</v>
       </c>
     </row>
+    <row r="701">
+      <c r="A701" s="27" t="n">
+        <v>45686</v>
+      </c>
+      <c r="C701" t="n">
+        <v>353.1000061035156</v>
+      </c>
+      <c r="D701" t="n">
+        <v>206.0399932861328</v>
+      </c>
+      <c r="E701" t="n">
+        <v>1029.650024414062</v>
+      </c>
+      <c r="F701" t="n">
+        <v>895.0999755859375</v>
+      </c>
+      <c r="G701" t="n">
+        <v>175.4900054931641</v>
+      </c>
+      <c r="H701" t="n">
+        <v>20981.91987609863</v>
+      </c>
+      <c r="I701" t="n">
+        <v>0.01148395685018959</v>
+      </c>
+      <c r="J701" t="n">
+        <v>199.5634713975556</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" s="27" t="n">
+        <v>45687</v>
+      </c>
+      <c r="C702" t="n">
+        <v>360</v>
+      </c>
+      <c r="D702" t="n">
+        <v>210.3300018310547</v>
+      </c>
+      <c r="E702" t="n">
+        <v>1027.300048828125</v>
+      </c>
+      <c r="F702" t="n">
+        <v>907.0499877929688</v>
+      </c>
+      <c r="G702" t="n">
+        <v>174.9299926757812</v>
+      </c>
+      <c r="H702" t="n">
+        <v>21274.5401763916</v>
+      </c>
+      <c r="I702" t="n">
+        <v>0.01394630720262661</v>
+      </c>
+      <c r="J702" t="n">
+        <v>202.3466448760885</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" s="27" t="n">
+        <v>45688</v>
+      </c>
+      <c r="C703" t="n">
+        <v>374.5</v>
+      </c>
+      <c r="D703" t="n">
+        <v>216.8300018310547</v>
+      </c>
+      <c r="E703" t="n">
+        <v>1034.949951171875</v>
+      </c>
+      <c r="F703" t="n">
+        <v>945.5999755859375</v>
+      </c>
+      <c r="G703" t="n">
+        <v>177.3800048828125</v>
+      </c>
+      <c r="H703" t="n">
+        <v>21936.28974914551</v>
+      </c>
+      <c r="I703" t="n">
+        <v>0.03110523504936906</v>
+      </c>
+      <c r="J703" t="n">
+        <v>208.6406848264104</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" s="27" t="n">
+        <v>45689</v>
+      </c>
+      <c r="C704" t="n">
+        <v>382.2999877929688</v>
+      </c>
+      <c r="D704" t="n">
+        <v>206.3500061035156</v>
+      </c>
+      <c r="E704" t="n">
+        <v>1077.300048828125</v>
+      </c>
+      <c r="F704" t="n">
+        <v>989.7999877929688</v>
+      </c>
+      <c r="G704" t="n">
+        <v>177.6300048828125</v>
+      </c>
+      <c r="H704" t="n">
+        <v>22127.11013793945</v>
+      </c>
+      <c r="I704" t="n">
+        <v>0.008698845200172394</v>
+      </c>
+      <c r="J704" t="n">
+        <v>210.4556178461733</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" s="27" t="n">
+        <v>45691</v>
+      </c>
+      <c r="C705" t="n">
+        <v>373.6499938964844</v>
+      </c>
+      <c r="D705" t="n">
+        <v>203.9100036621094</v>
+      </c>
+      <c r="E705" t="n">
+        <v>1067.800048828125</v>
+      </c>
+      <c r="F705" t="n">
+        <v>962.1500244140625</v>
+      </c>
+      <c r="G705" t="n">
+        <v>176.4700012207031</v>
+      </c>
+      <c r="H705" t="n">
+        <v>21734.50033569336</v>
+      </c>
+      <c r="I705" t="n">
+        <v>-0.01774338355974102</v>
+      </c>
+      <c r="J705" t="n">
+        <v>206.7214230964264</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" s="27" t="n">
+        <v>45692</v>
+      </c>
+      <c r="C706" t="n">
+        <v>380.25</v>
+      </c>
+      <c r="D706" t="n">
+        <v>211.6699981689453</v>
+      </c>
+      <c r="E706" t="n">
+        <v>1069.25</v>
+      </c>
+      <c r="F706" t="n">
+        <v>1001.5</v>
+      </c>
+      <c r="G706" t="n">
+        <v>187.8899993896484</v>
+      </c>
+      <c r="H706" t="n">
+        <v>22306.0499420166</v>
+      </c>
+      <c r="I706" t="n">
+        <v>0.02629688272081498</v>
+      </c>
+      <c r="J706" t="n">
+        <v>212.1575521154731</v>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" s="27" t="n">
+        <v>45693</v>
+      </c>
+      <c r="C707" t="n">
+        <v>384.8500061035156</v>
+      </c>
+      <c r="D707" t="n">
+        <v>211.0200042724609</v>
+      </c>
+      <c r="E707" t="n">
+        <v>1095</v>
+      </c>
+      <c r="F707" t="n">
+        <v>1024.300048828125</v>
+      </c>
+      <c r="G707" t="n">
+        <v>194.0399932861328</v>
+      </c>
+      <c r="H707" t="n">
+        <v>22588.80046081543</v>
+      </c>
+      <c r="I707" t="n">
+        <v>0.01267595650210697</v>
+      </c>
+      <c r="J707" t="n">
+        <v>214.8468520176823</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" s="27" t="n">
+        <v>45694</v>
+      </c>
+      <c r="C708" t="n">
+        <v>378.2000122070312</v>
+      </c>
+      <c r="D708" t="n">
+        <v>209.7899932861328</v>
+      </c>
+      <c r="E708" t="n">
+        <v>1087.400024414062</v>
+      </c>
+      <c r="F708" t="n">
+        <v>1030.150024414062</v>
+      </c>
+      <c r="G708" t="n">
+        <v>210.1000061035156</v>
+      </c>
+      <c r="H708" t="n">
+        <v>22475.24021911621</v>
+      </c>
+      <c r="I708" t="n">
+        <v>-0.005027280748980478</v>
+      </c>
+      <c r="J708" t="n">
+        <v>213.7667565745548</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" s="27" t="n">
+        <v>45695</v>
+      </c>
+      <c r="C709" t="n">
+        <v>377.1000061035156</v>
+      </c>
+      <c r="D709" t="n">
+        <v>212.0500030517578</v>
+      </c>
+      <c r="E709" t="n">
+        <v>1069.099975585938</v>
+      </c>
+      <c r="F709" t="n">
+        <v>1052.75</v>
+      </c>
+      <c r="G709" t="n">
+        <v>209.8000030517578</v>
+      </c>
+      <c r="H709" t="n">
+        <v>22566.90010070801</v>
+      </c>
+      <c r="I709" t="n">
+        <v>0.004078260374446899</v>
+      </c>
+      <c r="J709" t="n">
+        <v>214.6385530672668</v>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" s="27" t="n">
+        <v>45698</v>
+      </c>
+      <c r="C710" t="n">
+        <v>371.7000122070312</v>
+      </c>
+      <c r="D710" t="n">
+        <v>209.1000061035156</v>
+      </c>
+      <c r="E710" t="n">
+        <v>1031.75</v>
+      </c>
+      <c r="F710" t="n">
+        <v>1073.099975585938</v>
+      </c>
+      <c r="G710" t="n">
+        <v>210.4600067138672</v>
+      </c>
+      <c r="H710" t="n">
+        <v>22342.72027587891</v>
+      </c>
+      <c r="I710" t="n">
+        <v>-0.0099340106008653</v>
+      </c>
+      <c r="J710" t="n">
+        <v>212.5063314057422</v>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" s="27" t="n">
+        <v>45699</v>
+      </c>
+      <c r="C711" t="n">
+        <v>362.8999938964844</v>
+      </c>
+      <c r="D711" t="n">
+        <v>203.7100067138672</v>
+      </c>
+      <c r="E711" t="n">
+        <v>1000.799987792969</v>
+      </c>
+      <c r="F711" t="n">
+        <v>986.5</v>
+      </c>
+      <c r="G711" t="n">
+        <v>207.4299926757812</v>
+      </c>
+      <c r="H711" t="n">
+        <v>21471.97004699707</v>
+      </c>
+      <c r="I711" t="n">
+        <v>-0.03897243568062272</v>
+      </c>
+      <c r="J711" t="n">
+        <v>204.2244420733068</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" s="27" t="n">
+        <v>45700</v>
+      </c>
+      <c r="C712" t="n">
+        <v>365.7000122070312</v>
+      </c>
+      <c r="D712" t="n">
+        <v>219.3500061035156</v>
+      </c>
+      <c r="E712" t="n">
+        <v>1001.200012207031</v>
+      </c>
+      <c r="F712" t="n">
+        <v>990.5499877929688</v>
+      </c>
+      <c r="G712" t="n">
+        <v>207.1399993896484</v>
+      </c>
+      <c r="H712" t="n">
+        <v>22022.88037109375</v>
+      </c>
+      <c r="I712" t="n">
+        <v>0.02565718575849664</v>
+      </c>
+      <c r="J712" t="n">
+        <v>209.464266520007</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" s="27" t="n">
+        <v>45701</v>
+      </c>
+      <c r="C713" t="n">
+        <v>366.9500122070312</v>
+      </c>
+      <c r="D713" t="n">
+        <v>217.0700073242188</v>
+      </c>
+      <c r="E713" t="n">
+        <v>983.3499755859375</v>
+      </c>
+      <c r="F713" t="n">
+        <v>946.8499755859375</v>
+      </c>
+      <c r="G713" t="n">
+        <v>206.8200073242188</v>
+      </c>
+      <c r="H713" t="n">
+        <v>21681.66021728516</v>
+      </c>
+      <c r="I713" t="n">
+        <v>-0.01549389308114592</v>
+      </c>
+      <c r="J713" t="n">
+        <v>206.2188495702253</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" s="27" t="n">
+        <v>45702</v>
+      </c>
+      <c r="C714" t="n">
+        <v>358.5499877929688</v>
+      </c>
+      <c r="D714" t="n">
+        <v>213.8500061035156</v>
+      </c>
+      <c r="E714" t="n">
+        <v>954.3499755859375</v>
+      </c>
+      <c r="F714" t="n">
+        <v>906.25</v>
+      </c>
+      <c r="G714" t="n">
+        <v>196.6000061035156</v>
+      </c>
+      <c r="H714" t="n">
+        <v>21107.99990844727</v>
+      </c>
+      <c r="I714" t="n">
+        <v>-0.02645832021574411</v>
+      </c>
+      <c r="J714" t="n">
+        <v>200.7626452137739</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" s="27" t="n">
+        <v>45705</v>
+      </c>
+      <c r="C715" t="n">
+        <v>361.7999877929688</v>
+      </c>
+      <c r="D715" t="n">
+        <v>223.6100006103516</v>
+      </c>
+      <c r="E715" t="n">
+        <v>965.25</v>
+      </c>
+      <c r="F715" t="n">
+        <v>890.5499877929688</v>
+      </c>
+      <c r="G715" t="n">
+        <v>208.1199951171875</v>
+      </c>
+      <c r="H715" t="n">
+        <v>21450.69975280762</v>
+      </c>
+      <c r="I715" t="n">
+        <v>0.01623554319910744</v>
+      </c>
+      <c r="J715" t="n">
+        <v>204.0221358129093</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" s="27" t="n">
+        <v>45706</v>
+      </c>
+      <c r="C716" t="n">
+        <v>360.5499877929688</v>
+      </c>
+      <c r="D716" t="n">
+        <v>222.2799987792969</v>
+      </c>
+      <c r="E716" t="n">
+        <v>948.5999755859375</v>
+      </c>
+      <c r="F716" t="n">
+        <v>865.4000244140625</v>
+      </c>
+      <c r="G716" t="n">
+        <v>207.5500030517578</v>
+      </c>
+      <c r="H716" t="n">
+        <v>21195.97979736328</v>
+      </c>
+      <c r="I716" t="n">
+        <v>-0.01187466881638658</v>
+      </c>
+      <c r="J716" t="n">
+        <v>201.5994405189191</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" s="27" t="n">
+        <v>45707</v>
+      </c>
+      <c r="C717" t="n">
+        <v>364.0499877929688</v>
+      </c>
+      <c r="D717" t="n">
+        <v>225.4100036621094</v>
+      </c>
+      <c r="E717" t="n">
+        <v>970.8499755859375</v>
+      </c>
+      <c r="F717" t="n">
+        <v>850.2000122070312</v>
+      </c>
+      <c r="G717" t="n">
+        <v>207.6799926757812</v>
+      </c>
+      <c r="H717" t="n">
+        <v>21362.26986694336</v>
+      </c>
+      <c r="I717" t="n">
+        <v>0.007845358939281691</v>
+      </c>
+      <c r="J717" t="n">
+        <v>203.1810604917484</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" s="27" t="n">
+        <v>45708</v>
+      </c>
+      <c r="C718" t="n">
+        <v>374.9500122070312</v>
+      </c>
+      <c r="D718" t="n">
+        <v>226.4900054931641</v>
+      </c>
+      <c r="E718" t="n">
+        <v>1044.650024414062</v>
+      </c>
+      <c r="F718" t="n">
+        <v>869.3499755859375</v>
+      </c>
+      <c r="G718" t="n">
+        <v>213.9600067138672</v>
+      </c>
+      <c r="H718" t="n">
+        <v>21973.66035461426</v>
+      </c>
+      <c r="I718" t="n">
+        <v>0.02862010879363448</v>
+      </c>
+      <c r="J718" t="n">
+        <v>208.9961245478283</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" s="27" t="n">
+        <v>45709</v>
+      </c>
+      <c r="C719" t="n">
+        <v>365.2999877929688</v>
+      </c>
+      <c r="D719" t="n">
+        <v>222.5299987792969</v>
+      </c>
+      <c r="E719" t="n">
+        <v>1015.349975585938</v>
+      </c>
+      <c r="F719" t="n">
+        <v>853.0999755859375</v>
+      </c>
+      <c r="G719" t="n">
+        <v>215.4199981689453</v>
+      </c>
+      <c r="H719" t="n">
+        <v>21500.96954345703</v>
+      </c>
+      <c r="I719" t="n">
+        <v>-0.02151170098785867</v>
+      </c>
+      <c r="J719" t="n">
+        <v>204.5002624089341</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" s="27" t="n">
+        <v>45712</v>
+      </c>
+      <c r="C720" t="n">
+        <v>364.5</v>
+      </c>
+      <c r="D720" t="n">
+        <v>223.0899963378906</v>
+      </c>
+      <c r="E720" t="n">
+        <v>1007.400024414062</v>
+      </c>
+      <c r="F720" t="n">
+        <v>849.2000122070312</v>
+      </c>
+      <c r="G720" t="n">
+        <v>214.4700012207031</v>
+      </c>
+      <c r="H720" t="n">
+        <v>21452.33004760742</v>
+      </c>
+      <c r="I720" t="n">
+        <v>-0.002262200118524928</v>
+      </c>
+      <c r="J720" t="n">
+        <v>204.0376418910742</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" s="27" t="n">
+        <v>45713</v>
+      </c>
+      <c r="C721" t="n">
+        <v>363.8500061035156</v>
+      </c>
+      <c r="D721" t="n">
+        <v>227.2299957275391</v>
+      </c>
+      <c r="E721" t="n">
+        <v>1046.449951171875</v>
+      </c>
+      <c r="F721" t="n">
+        <v>853.0999755859375</v>
+      </c>
+      <c r="G721" t="n">
+        <v>217.3200073242188</v>
+      </c>
+      <c r="H721" t="n">
+        <v>21751.66966247559</v>
+      </c>
+      <c r="I721" t="n">
+        <v>0.01395371105161369</v>
+      </c>
+      <c r="J721" t="n">
+        <v>206.8847241896749</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" s="27" t="n">
+        <v>45715</v>
+      </c>
+      <c r="C722" t="n">
+        <v>354.5</v>
+      </c>
+      <c r="D722" t="n">
+        <v>225.4299926757812</v>
+      </c>
+      <c r="E722" t="n">
+        <v>997.75</v>
+      </c>
+      <c r="F722" t="n">
+        <v>829.2999877929688</v>
+      </c>
+      <c r="G722" t="n">
+        <v>218.4700012207031</v>
+      </c>
+      <c r="H722" t="n">
+        <v>21234.76971435547</v>
+      </c>
+      <c r="I722" t="n">
+        <v>-0.02376369061046545</v>
+      </c>
+      <c r="J722" t="n">
+        <v>201.968379612</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" s="27" t="n">
+        <v>45716</v>
+      </c>
+      <c r="C723" t="n">
+        <v>347.7999877929688</v>
+      </c>
+      <c r="D723" t="n">
+        <v>212.9400024414062</v>
+      </c>
+      <c r="E723" t="n">
+        <v>979.9500122070312</v>
+      </c>
+      <c r="F723" t="n">
+        <v>825.9000244140625</v>
+      </c>
+      <c r="G723" t="n">
+        <v>212.6300048828125</v>
+      </c>
+      <c r="H723" t="n">
+        <v>20640.50006103516</v>
+      </c>
+      <c r="I723" t="n">
+        <v>-0.02798568862833322</v>
+      </c>
+      <c r="J723" t="n">
+        <v>196.3161554274095</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" s="27" t="n">
+        <v>45719</v>
+      </c>
+      <c r="C724" t="n">
+        <v>346.2999877929688</v>
+      </c>
+      <c r="D724" t="n">
+        <v>208.9199981689453</v>
+      </c>
+      <c r="E724" t="n">
+        <v>947.7000122070312</v>
+      </c>
+      <c r="F724" t="n">
+        <v>828.5999755859375</v>
+      </c>
+      <c r="G724" t="n">
+        <v>217.3399963378906</v>
+      </c>
+      <c r="H724" t="n">
+        <v>20385.7996673584</v>
+      </c>
+      <c r="I724" t="n">
+        <v>-0.01233983638592059</v>
+      </c>
+      <c r="J724" t="n">
+        <v>193.8936461895223</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" s="27" t="n">
+        <v>45720</v>
+      </c>
+      <c r="C725" t="n">
+        <v>345.7000122070312</v>
+      </c>
+      <c r="D725" t="n">
+        <v>206.9299926757812</v>
+      </c>
+      <c r="E725" t="n">
+        <v>965.5999755859375</v>
+      </c>
+      <c r="F725" t="n">
+        <v>835.0499877929688</v>
+      </c>
+      <c r="G725" t="n">
+        <v>222.0399932861328</v>
+      </c>
+      <c r="H725" t="n">
+        <v>20427.75979614258</v>
+      </c>
+      <c r="I725" t="n">
+        <v>0.002058301831120511</v>
+      </c>
+      <c r="J725" t="n">
+        <v>194.2927378365169</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" s="27" t="n">
+        <v>45721</v>
+      </c>
+      <c r="C726" t="n">
+        <v>356.3999938964844</v>
+      </c>
+      <c r="D726" t="n">
+        <v>209.2100067138672</v>
+      </c>
+      <c r="E726" t="n">
+        <v>1000.950012207031</v>
+      </c>
+      <c r="F726" t="n">
+        <v>853.5</v>
+      </c>
+      <c r="G726" t="n">
+        <v>222.3300018310547</v>
+      </c>
+      <c r="H726" t="n">
+        <v>20903.87016296387</v>
+      </c>
+      <c r="I726" t="n">
+        <v>0.02330702786661874</v>
+      </c>
+      <c r="J726" t="n">
+        <v>198.8211240915542</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" s="27" t="n">
+        <v>45722</v>
+      </c>
+      <c r="C727" t="n">
+        <v>355.5</v>
+      </c>
+      <c r="D727" t="n">
+        <v>210.6000061035156</v>
+      </c>
+      <c r="E727" t="n">
+        <v>1003.75</v>
+      </c>
+      <c r="F727" t="n">
+        <v>870.9500122070312</v>
+      </c>
+      <c r="G727" t="n">
+        <v>245.8800048828125</v>
+      </c>
+      <c r="H727" t="n">
+        <v>21078.11026000977</v>
+      </c>
+      <c r="I727" t="n">
+        <v>0.008335303256647941</v>
+      </c>
+      <c r="J727" t="n">
+        <v>200.478358454685</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" s="27" t="n">
+        <v>45723</v>
+      </c>
+      <c r="C728" t="n">
+        <v>355.8500061035156</v>
+      </c>
+      <c r="D728" t="n">
+        <v>209.7799987792969</v>
+      </c>
+      <c r="E728" t="n">
+        <v>998.7999877929688</v>
+      </c>
+      <c r="F728" t="n">
+        <v>870.6500244140625</v>
+      </c>
+      <c r="G728" t="n">
+        <v>240.6699981689453</v>
+      </c>
+      <c r="H728" t="n">
+        <v>21026.57012939453</v>
+      </c>
+      <c r="I728" t="n">
+        <v>-0.002445196935562975</v>
+      </c>
+      <c r="J728" t="n">
+        <v>199.9881493869449</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" s="27" t="n">
+        <v>45726</v>
+      </c>
+      <c r="C729" t="n">
+        <v>346.8999938964844</v>
+      </c>
+      <c r="D729" t="n">
+        <v>206.7899932861328</v>
+      </c>
+      <c r="E729" t="n">
+        <v>998.6500244140625</v>
+      </c>
+      <c r="F729" t="n">
+        <v>855.75</v>
+      </c>
+      <c r="G729" t="n">
+        <v>234.8099975585938</v>
+      </c>
+      <c r="H729" t="n">
+        <v>20703.8597869873</v>
+      </c>
+      <c r="I729" t="n">
+        <v>-0.01534774052169768</v>
+      </c>
+      <c r="J729" t="n">
+        <v>196.9187831627395</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" s="27" t="n">
+        <v>45727</v>
+      </c>
+      <c r="C730" t="n">
+        <v>344.6000061035156</v>
+      </c>
+      <c r="D730" t="n">
+        <v>199.9600067138672</v>
+      </c>
+      <c r="E730" t="n">
+        <v>987.3499755859375</v>
+      </c>
+      <c r="F730" t="n">
+        <v>855.4000244140625</v>
+      </c>
+      <c r="G730" t="n">
+        <v>241.3699951171875</v>
+      </c>
+      <c r="H730" t="n">
+        <v>20421.50032043457</v>
+      </c>
+      <c r="I730" t="n">
+        <v>-0.01363801095340694</v>
+      </c>
+      <c r="J730" t="n">
+        <v>194.2332026410345</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" s="27" t="n">
+        <v>45728</v>
+      </c>
+      <c r="C731" t="n">
+        <v>340.6499938964844</v>
+      </c>
+      <c r="D731" t="n">
+        <v>196.1100006103516</v>
+      </c>
+      <c r="E731" t="n">
+        <v>977.5499877929688</v>
+      </c>
+      <c r="F731" t="n">
+        <v>860.7000122070312</v>
+      </c>
+      <c r="G731" t="n">
+        <v>239.9199981689453</v>
+      </c>
+      <c r="H731" t="n">
+        <v>20223.34992980957</v>
+      </c>
+      <c r="I731" t="n">
+        <v>-0.009703028059438061</v>
+      </c>
+      <c r="J731" t="n">
+        <v>192.3485524257341</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" s="27" t="n">
+        <v>45729</v>
+      </c>
+      <c r="C732" t="n">
+        <v>333</v>
+      </c>
+      <c r="D732" t="n">
+        <v>196.6300048828125</v>
+      </c>
+      <c r="E732" t="n">
+        <v>961.6500244140625</v>
+      </c>
+      <c r="F732" t="n">
+        <v>902.8499755859375</v>
+      </c>
+      <c r="G732" t="n">
+        <v>231.0800018310547</v>
+      </c>
+      <c r="H732" t="n">
+        <v>20246.54013061523</v>
+      </c>
+      <c r="I732" t="n">
+        <v>0.00114670422487628</v>
+      </c>
+      <c r="J732" t="n">
+        <v>192.5691193234495</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" s="27" t="n">
+        <v>45733</v>
+      </c>
+      <c r="C733" t="n">
+        <v>334.1499938964844</v>
+      </c>
+      <c r="D733" t="n">
+        <v>198.4600067138672</v>
+      </c>
+      <c r="E733" t="n">
+        <v>970.0999755859375</v>
+      </c>
+      <c r="F733" t="n">
+        <v>935.5</v>
+      </c>
+      <c r="G733" t="n">
+        <v>236.0200042724609</v>
+      </c>
+      <c r="H733" t="n">
+        <v>20528.6000213623</v>
+      </c>
+      <c r="I733" t="n">
+        <v>0.01393126375802656</v>
+      </c>
+      <c r="J733" t="n">
+        <v>195.2518505163953</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" s="27" t="n">
+        <v>45734</v>
+      </c>
+      <c r="C734" t="n">
+        <v>334.1499938964844</v>
+      </c>
+      <c r="D734" t="n">
+        <v>198.4600067138672</v>
+      </c>
+      <c r="E734" t="n">
+        <v>1006</v>
+      </c>
+      <c r="F734" t="n">
+        <v>935.5</v>
+      </c>
+      <c r="G734" t="n">
+        <v>236.0200042724609</v>
+      </c>
+      <c r="H734" t="n">
+        <v>20672.20011901855</v>
+      </c>
+      <c r="I734" t="n">
+        <v>0.006995123754509223</v>
+      </c>
+      <c r="J734" t="n">
+        <v>196.6176613740544</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" s="27" t="n">
+        <v>45735</v>
+      </c>
+      <c r="C735" t="n">
+        <v>350.1499938964844</v>
+      </c>
+      <c r="D735" t="n">
+        <v>205.6900024414062</v>
+      </c>
+      <c r="E735" t="n">
+        <v>1060</v>
+      </c>
+      <c r="F735" t="n">
+        <v>1012.549987792969</v>
+      </c>
+      <c r="G735" t="n">
+        <v>218.7799987792969</v>
+      </c>
+      <c r="H735" t="n">
+        <v>21719.09991455078</v>
+      </c>
+      <c r="I735" t="n">
+        <v>0.05064288220435096</v>
+      </c>
+      <c r="J735" t="n">
+        <v>206.5749464383157</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" s="27" t="n">
+        <v>45736</v>
+      </c>
+      <c r="C736" t="n">
+        <v>355.6499938964844</v>
+      </c>
+      <c r="D736" t="n">
+        <v>207.4799957275391</v>
+      </c>
+      <c r="E736" t="n">
+        <v>1038.5</v>
+      </c>
+      <c r="F736" t="n">
+        <v>978.2999877929688</v>
+      </c>
+      <c r="G736" t="n">
+        <v>216.3899993896484</v>
+      </c>
+      <c r="H736" t="n">
+        <v>21600.5597076416</v>
+      </c>
+      <c r="I736" t="n">
+        <v>-0.005457878428459335</v>
+      </c>
+      <c r="J736" t="n">
+        <v>205.4474854942898</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" s="27" t="n">
+        <v>45737</v>
+      </c>
+      <c r="C737" t="n">
+        <v>358.6499938964844</v>
+      </c>
+      <c r="D737" t="n">
+        <v>210.8399963378906</v>
+      </c>
+      <c r="E737" t="n">
+        <v>1063.199951171875</v>
+      </c>
+      <c r="F737" t="n">
+        <v>974.0999755859375</v>
+      </c>
+      <c r="G737" t="n">
+        <v>217.4700012207031</v>
+      </c>
+      <c r="H737" t="n">
+        <v>21832.67947387695</v>
+      </c>
+      <c r="I737" t="n">
+        <v>0.01074600701912529</v>
+      </c>
+      <c r="J737" t="n">
+        <v>207.6552256154731</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" s="27" t="n">
+        <v>45740</v>
+      </c>
+      <c r="C738" t="n">
+        <v>366</v>
+      </c>
+      <c r="D738" t="n">
+        <v>212.5299987792969</v>
+      </c>
+      <c r="E738" t="n">
+        <v>1069.800048828125</v>
+      </c>
+      <c r="F738" t="n">
+        <v>951.75</v>
+      </c>
+      <c r="G738" t="n">
+        <v>219.2899932861328</v>
+      </c>
+      <c r="H738" t="n">
+        <v>21920.96014404297</v>
+      </c>
+      <c r="I738" t="n">
+        <v>0.004043510567342155</v>
+      </c>
+      <c r="J738" t="n">
+        <v>208.4948817146131</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" s="27" t="n">
+        <v>45741</v>
+      </c>
+      <c r="C739" t="n">
+        <v>360.2000122070312</v>
+      </c>
+      <c r="D739" t="n">
+        <v>210.0399932861328</v>
+      </c>
+      <c r="E739" t="n">
+        <v>1054.550048828125</v>
+      </c>
+      <c r="F739" t="n">
+        <v>941.5499877929688</v>
+      </c>
+      <c r="G739" t="n">
+        <v>208.4900054931641</v>
+      </c>
+      <c r="H739" t="n">
+        <v>21617.37013244629</v>
+      </c>
+      <c r="I739" t="n">
+        <v>-0.01384930265835917</v>
+      </c>
+      <c r="J739" t="n">
+        <v>205.6073729950286</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" s="27" t="n">
+        <v>45742</v>
+      </c>
+      <c r="C740" t="n">
+        <v>359.1000061035156</v>
+      </c>
+      <c r="D740" t="n">
+        <v>214.9799957275391</v>
+      </c>
+      <c r="E740" t="n">
+        <v>1040.900024414062</v>
+      </c>
+      <c r="F740" t="n">
+        <v>934.4500122070312</v>
+      </c>
+      <c r="G740" t="n">
+        <v>205.6799926757812</v>
+      </c>
+      <c r="H740" t="n">
+        <v>21657.19010925293</v>
+      </c>
+      <c r="I740" t="n">
+        <v>0.001842036129402873</v>
+      </c>
+      <c r="J740" t="n">
+        <v>205.9861092045571</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" s="27" t="n">
+        <v>45743</v>
+      </c>
+      <c r="C741" t="n">
+        <v>360.0499877929688</v>
+      </c>
+      <c r="D741" t="n">
+        <v>208.5200042724609</v>
+      </c>
+      <c r="E741" t="n">
+        <v>1024.25</v>
+      </c>
+      <c r="F741" t="n">
+        <v>915.9000244140625</v>
+      </c>
+      <c r="G741" t="n">
+        <v>208.9700012207031</v>
+      </c>
+      <c r="H741" t="n">
+        <v>21319.36006164551</v>
+      </c>
+      <c r="I741" t="n">
+        <v>-0.01559897871806951</v>
+      </c>
+      <c r="J741" t="n">
+        <v>202.7729362708573</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" s="27" t="n">
+        <v>45744</v>
+      </c>
+      <c r="C742" t="n">
+        <v>360.4500122070312</v>
+      </c>
+      <c r="D742" t="n">
+        <v>204.2200012207031</v>
+      </c>
+      <c r="E742" t="n">
+        <v>1003</v>
+      </c>
+      <c r="F742" t="n">
+        <v>875.5</v>
+      </c>
+      <c r="G742" t="n">
+        <v>202.9600067138672</v>
+      </c>
+      <c r="H742" t="n">
+        <v>20893.44024658203</v>
+      </c>
+      <c r="I742" t="n">
+        <v>-0.01997807691374966</v>
+      </c>
+      <c r="J742" t="n">
+        <v>198.7219229540112</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" s="27" t="n">
+        <v>45748</v>
+      </c>
+      <c r="C743" t="n">
+        <v>364.7999877929688</v>
+      </c>
+      <c r="D743" t="n">
+        <v>209.0599975585938</v>
+      </c>
+      <c r="E743" t="n">
+        <v>1014.799987792969</v>
+      </c>
+      <c r="F743" t="n">
+        <v>890.1500244140625</v>
+      </c>
+      <c r="G743" t="n">
+        <v>206.8600006103516</v>
+      </c>
+      <c r="H743" t="n">
+        <v>21241.3298034668</v>
+      </c>
+      <c r="I743" t="n">
+        <v>0.01665065938299352</v>
+      </c>
+      <c r="J743" t="n">
+        <v>202.0307740050519</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" s="27" t="n">
+        <v>45749</v>
+      </c>
+      <c r="C744" t="n">
+        <v>371.6000061035156</v>
+      </c>
+      <c r="D744" t="n">
+        <v>208.7700042724609</v>
+      </c>
+      <c r="E744" t="n">
+        <v>1030.599975585938</v>
+      </c>
+      <c r="F744" t="n">
+        <v>881.7999877929688</v>
+      </c>
+      <c r="G744" t="n">
+        <v>202.7899932861328</v>
+      </c>
+      <c r="H744" t="n">
+        <v>21354.4500579834</v>
+      </c>
+      <c r="I744" t="n">
+        <v>0.005325478939559576</v>
+      </c>
+      <c r="J744" t="n">
+        <v>203.1066846371588</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" s="27" t="n">
+        <v>45750</v>
+      </c>
+      <c r="C745" t="n">
+        <v>372.2000122070312</v>
+      </c>
+      <c r="D745" t="n">
+        <v>209.9400024414062</v>
+      </c>
+      <c r="E745" t="n">
+        <v>1014.349975585938</v>
+      </c>
+      <c r="F745" t="n">
+        <v>863.7000122070312</v>
+      </c>
+      <c r="G745" t="n">
+        <v>200.9400024414062</v>
+      </c>
+      <c r="H745" t="n">
+        <v>21241.12023925781</v>
+      </c>
+      <c r="I745" t="n">
+        <v>-0.005307082056333143</v>
+      </c>
+      <c r="J745" t="n">
+        <v>202.0287807955996</v>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" s="27" t="n">
+        <v>45751</v>
+      </c>
+      <c r="C746" t="n">
+        <v>364.3999938964844</v>
+      </c>
+      <c r="D746" t="n">
+        <v>205.1399993896484</v>
+      </c>
+      <c r="E746" t="n">
+        <v>991.25</v>
+      </c>
+      <c r="F746" t="n">
+        <v>830.75</v>
+      </c>
+      <c r="G746" t="n">
+        <v>203.2799987792969</v>
+      </c>
+      <c r="H746" t="n">
+        <v>20715.04988098145</v>
+      </c>
+      <c r="I746" t="n">
+        <v>-0.02476660140099789</v>
+      </c>
+      <c r="J746" t="n">
+        <v>197.0252145101054</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" s="27" t="n">
+        <v>45754</v>
+      </c>
+      <c r="C747" t="n">
+        <v>353.3999938964844</v>
+      </c>
+      <c r="D747" t="n">
+        <v>197.5899963378906</v>
+      </c>
+      <c r="E747" t="n">
+        <v>955.2999877929688</v>
+      </c>
+      <c r="F747" t="n">
+        <v>802.8499755859375</v>
+      </c>
+      <c r="G747" t="n">
+        <v>198.5700073242188</v>
+      </c>
+      <c r="H747" t="n">
+        <v>20012.27963256836</v>
+      </c>
+      <c r="I747" t="n">
+        <v>-0.03392558803627606</v>
+      </c>
+      <c r="J747" t="n">
+        <v>190.3410182498767</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" s="27" t="n">
+        <v>45755</v>
+      </c>
+      <c r="C748" t="n">
+        <v>357.6499938964844</v>
+      </c>
+      <c r="D748" t="n">
+        <v>201.8200073242188</v>
+      </c>
+      <c r="E748" t="n">
+        <v>967.5</v>
+      </c>
+      <c r="F748" t="n">
+        <v>837.2999877929688</v>
+      </c>
+      <c r="G748" t="n">
+        <v>193.5200042724609</v>
+      </c>
+      <c r="H748" t="n">
+        <v>20422.3600769043</v>
+      </c>
+      <c r="I748" t="n">
+        <v>0.02049144084857604</v>
+      </c>
+      <c r="J748" t="n">
+        <v>194.2413799664018</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" s="27" t="n">
+        <v>45756</v>
+      </c>
+      <c r="C749" t="n">
+        <v>364.3500061035156</v>
+      </c>
+      <c r="D749" t="n">
+        <v>204.6799926757812</v>
+      </c>
+      <c r="E749" t="n">
+        <v>968.4000244140625</v>
+      </c>
+      <c r="F749" t="n">
+        <v>814.7999877929688</v>
+      </c>
+      <c r="G749" t="n">
+        <v>196.1600036621094</v>
+      </c>
+      <c r="H749" t="n">
+        <v>20514.59991455078</v>
+      </c>
+      <c r="I749" t="n">
+        <v>0.004516610093012642</v>
+      </c>
+      <c r="J749" t="n">
+        <v>195.1186925436387</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" s="27" t="n">
+        <v>45758</v>
+      </c>
+      <c r="C750" t="n">
+        <v>369.2999877929688</v>
+      </c>
+      <c r="D750" t="n">
+        <v>208.5</v>
+      </c>
+      <c r="E750" t="n">
+        <v>975.3499755859375</v>
+      </c>
+      <c r="F750" t="n">
+        <v>824.1500244140625</v>
+      </c>
+      <c r="G750" t="n">
+        <v>199.3300018310547</v>
+      </c>
+      <c r="H750" t="n">
+        <v>20793.10983276367</v>
+      </c>
+      <c r="I750" t="n">
+        <v>0.01357618083574453</v>
+      </c>
+      <c r="J750" t="n">
+        <v>197.7676591980452</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" s="27" t="n">
+        <v>45762</v>
+      </c>
+      <c r="C751" t="n">
+        <v>379.7000122070312</v>
+      </c>
+      <c r="D751" t="n">
+        <v>214.9499969482422</v>
+      </c>
+      <c r="E751" t="n">
+        <v>994.5499877929688</v>
+      </c>
+      <c r="F751" t="n">
+        <v>877.9000244140625</v>
+      </c>
+      <c r="G751" t="n">
+        <v>203.8999938964844</v>
+      </c>
+      <c r="H751" t="n">
+        <v>21514.15016174316</v>
+      </c>
+      <c r="I751" t="n">
+        <v>0.03467688742947676</v>
+      </c>
+      <c r="J751" t="n">
+        <v>204.625626053247</v>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" s="27" t="n">
+        <v>45763</v>
+      </c>
+      <c r="C752" t="n">
+        <v>377</v>
+      </c>
+      <c r="D752" t="n">
+        <v>214.3999938964844</v>
+      </c>
+      <c r="E752" t="n">
+        <v>995.25</v>
+      </c>
+      <c r="F752" t="n">
+        <v>852.9500122070312</v>
+      </c>
+      <c r="G752" t="n">
+        <v>206.0299987792969</v>
+      </c>
+      <c r="H752" t="n">
+        <v>21336.20986938477</v>
+      </c>
+      <c r="I752" t="n">
+        <v>-0.008270849232744269</v>
+      </c>
+      <c r="J752" t="n">
+        <v>202.9331983510047</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" s="27" t="n">
+        <v>45764</v>
+      </c>
+      <c r="C753" t="n">
+        <v>375.2999877929688</v>
+      </c>
+      <c r="D753" t="n">
+        <v>218.9799957275391</v>
+      </c>
+      <c r="E753" t="n">
+        <v>1019.700012207031</v>
+      </c>
+      <c r="F753" t="n">
+        <v>874.1500244140625</v>
+      </c>
+      <c r="G753" t="n">
+        <v>202.1199951171875</v>
+      </c>
+      <c r="H753" t="n">
+        <v>21646.96983337402</v>
+      </c>
+      <c r="I753" t="n">
+        <v>0.0145649094141676</v>
+      </c>
+      <c r="J753" t="n">
+        <v>205.8889020021143</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" s="27" t="n">
+        <v>45768</v>
+      </c>
+      <c r="C754" t="n">
+        <v>383.8999938964844</v>
+      </c>
+      <c r="D754" t="n">
+        <v>222.0599975585938</v>
+      </c>
+      <c r="E754" t="n">
+        <v>1033.699951171875</v>
+      </c>
+      <c r="F754" t="n">
+        <v>901.25</v>
+      </c>
+      <c r="G754" t="n">
+        <v>206.0399932861328</v>
+      </c>
+      <c r="H754" t="n">
+        <v>22079.38961791992</v>
+      </c>
+      <c r="I754" t="n">
+        <v>0.01997599608048694</v>
+      </c>
+      <c r="J754" t="n">
+        <v>210.0017379015243</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" s="27" t="n">
+        <v>45769</v>
+      </c>
+      <c r="C755" t="n">
+        <v>380.9500122070312</v>
+      </c>
+      <c r="D755" t="n">
+        <v>222.6699981689453</v>
+      </c>
+      <c r="E755" t="n">
+        <v>1015.900024414062</v>
+      </c>
+      <c r="F755" t="n">
+        <v>897.0999755859375</v>
+      </c>
+      <c r="G755" t="n">
+        <v>208.2700042724609</v>
+      </c>
+      <c r="H755" t="n">
+        <v>21963.61012268066</v>
+      </c>
+      <c r="I755" t="n">
+        <v>-0.005243781519453312</v>
+      </c>
+      <c r="J755" t="n">
+        <v>208.9005346692633</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" s="27" t="n">
+        <v>45770</v>
+      </c>
+      <c r="C756" t="n">
+        <v>380.7999877929688</v>
+      </c>
+      <c r="D756" t="n">
+        <v>230.6799926757812</v>
+      </c>
+      <c r="E756" t="n">
+        <v>1009.650024414062</v>
+      </c>
+      <c r="F756" t="n">
+        <v>904.25</v>
+      </c>
+      <c r="G756" t="n">
+        <v>208.4499969482422</v>
+      </c>
+      <c r="H756" t="n">
+        <v>22220.62966918945</v>
+      </c>
+      <c r="I756" t="n">
+        <v>0.01170206287004605</v>
+      </c>
+      <c r="J756" t="n">
+        <v>211.3451018595492</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" s="27" t="n">
+        <v>45771</v>
+      </c>
+      <c r="C757" t="n">
+        <v>382.4500122070312</v>
+      </c>
+      <c r="D757" t="n">
+        <v>230.6199951171875</v>
+      </c>
+      <c r="E757" t="n">
+        <v>1001.400024414062</v>
+      </c>
+      <c r="F757" t="n">
+        <v>895.5499877929688</v>
+      </c>
+      <c r="G757" t="n">
+        <v>208.6699981689453</v>
+      </c>
+      <c r="H757" t="n">
+        <v>22169.1100769043</v>
+      </c>
+      <c r="I757" t="n">
+        <v>-0.002318547811297714</v>
+      </c>
+      <c r="J757" t="n">
+        <v>210.8550881362043</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" s="27" t="n">
+        <v>45772</v>
+      </c>
+      <c r="C758" t="n">
+        <v>370.5</v>
+      </c>
+      <c r="D758" t="n">
+        <v>225.0399932861328</v>
+      </c>
+      <c r="E758" t="n">
+        <v>989.3499755859375</v>
+      </c>
+      <c r="F758" t="n">
+        <v>892.0499877929688</v>
+      </c>
+      <c r="G758" t="n">
+        <v>202.9799957275391</v>
+      </c>
+      <c r="H758" t="n">
+        <v>21727.84962463379</v>
+      </c>
+      <c r="I758" t="n">
+        <v>-0.01990429253766986</v>
+      </c>
+      <c r="J758" t="n">
+        <v>206.6581667788851</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" s="27" t="n">
+        <v>45775</v>
+      </c>
+      <c r="C759" t="n">
+        <v>377.2999877929688</v>
+      </c>
+      <c r="D759" t="n">
+        <v>227.4600067138672</v>
+      </c>
+      <c r="E759" t="n">
+        <v>984.6500244140625</v>
+      </c>
+      <c r="F759" t="n">
+        <v>883.7000122070312</v>
+      </c>
+      <c r="G759" t="n">
+        <v>209.5099945068359</v>
+      </c>
+      <c r="H759" t="n">
+        <v>21864.18016052246</v>
+      </c>
+      <c r="I759" t="n">
+        <v>0.006274460576812356</v>
+      </c>
+      <c r="J759" t="n">
+        <v>207.9548352992155</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>